<commit_message>
Changed Excel format from XLS to XLSX
</commit_message>
<xml_diff>
--- a/src/test/resources/config/working.xlsx
+++ b/src/test/resources/config/working.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d044854/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d065364/git/ma/cloud-realspend-expenses-uploader/src/test/resources/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19220" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Center Actuals" sheetId="1" r:id="rId1"/>
@@ -88,6 +88,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;€&quot;#,##0.00;[Red]\-&quot;€&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -153,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -161,9 +164,10 @@
     <xf numFmtId="4" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -440,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -574,13 +578,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:E4"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -610,8 +616,8 @@
       <c r="C2" s="3">
         <v>1104340</v>
       </c>
-      <c r="D2" s="3">
-        <v>200</v>
+      <c r="D2" s="4">
+        <v>4000000</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>8</v>
@@ -627,8 +633,8 @@
       <c r="C3" s="3">
         <v>1104341</v>
       </c>
-      <c r="D3" s="3">
-        <v>300</v>
+      <c r="D3" s="5">
+        <v>5000000</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
@@ -644,8 +650,8 @@
       <c r="C4" s="3">
         <v>1104342</v>
       </c>
-      <c r="D4" s="3">
-        <v>100</v>
+      <c r="D4" s="7">
+        <v>100000</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>8</v>
@@ -661,7 +667,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:E4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added overall budget posting, changed the log format, small fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/config/working.xlsx
+++ b/src/test/resources/config/working.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Center Actuals" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="16">
   <si>
     <t>User</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>EUR</t>
-  </si>
-  <si>
-    <t>100.000,00 €</t>
   </si>
   <si>
     <t>Account</t>
@@ -442,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,18 +475,22 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1104341</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1104341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="3">
         <v>1104342</v>
       </c>
     </row>
@@ -503,7 +504,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -562,8 +563,8 @@
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
+      <c r="C4" s="7">
+        <v>200000</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -578,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -769,10 +770,10 @@
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>6</v>
@@ -789,10 +790,10 @@
         <v>3</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F15" s="3">
         <v>200</v>
@@ -809,10 +810,10 @@
         <v>3</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="3">
         <v>300</v>
@@ -829,10 +830,10 @@
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="3">
         <v>100</v>
@@ -857,10 +858,10 @@
         <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F19" s="3">
         <v>1000</v>
@@ -877,10 +878,10 @@
         <v>4</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20" s="3">
         <v>5000</v>
@@ -897,10 +898,10 @@
         <v>4</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" s="3">
         <v>100</v>
@@ -925,10 +926,10 @@
         <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F23" s="3">
         <v>900</v>
@@ -945,10 +946,10 @@
         <v>2</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24" s="3">
         <v>700</v>
@@ -965,10 +966,10 @@
         <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" s="3">
         <v>300</v>

</xml_diff>